<commit_message>
Admin & Style général
Réattribution des couleurs du root css
Modification du  border-radius --> 13px
</commit_message>
<xml_diff>
--- a/Fonctionnalités.xlsx
+++ b/Fonctionnalités.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\biblio_version2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B238FFDD-C746-40AA-8F54-F6F00CBFAFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB58BC5B-336F-4803-8A2D-BD6B5565024C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F6FA006A-806B-4DC8-8CB4-F2137BEA4A1B}"/>
   </bookViews>
@@ -473,19 +473,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,13 +835,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE663369-7902-496D-9288-3154DCCCED76}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="61.1328125" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" customWidth="1"/>
     <col min="3" max="3" width="76.19921875" customWidth="1"/>
     <col min="4" max="4" width="11.265625" customWidth="1"/>
   </cols>
@@ -861,8 +861,8 @@
       </c>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -876,7 +876,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="20"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="13" t="s">
         <v>22</v>
       </c>
@@ -888,7 +888,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="20"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="13" t="s">
         <v>39</v>
       </c>
@@ -898,7 +898,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="20"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="13" t="s">
         <v>32</v>
       </c>
@@ -984,7 +984,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -998,7 +998,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="22"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="16" t="s">
         <v>8</v>
       </c>
@@ -1010,7 +1010,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="22"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="16" t="s">
         <v>9</v>
       </c>
@@ -1022,7 +1022,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="22"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="16" t="s">
         <v>10</v>
       </c>
@@ -1034,7 +1034,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="22"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="16" t="s">
         <v>35</v>
       </c>
@@ -1046,7 +1046,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="22"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="16" t="s">
         <v>34</v>
       </c>
@@ -1058,7 +1058,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="23"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>

</xml_diff>